<commit_message>
adding info regarding data acquisition
</commit_message>
<xml_diff>
--- a/csvFiles/metadata.xlsx
+++ b/csvFiles/metadata.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Chapter-4-Analyses\csvFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Chapter-2-Analyses\csvFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4143989E-EDB9-4FC2-BD4F-C3861766E5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE07555-415F-4BF6-BE1D-1E5C88E3FF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="555" windowWidth="29040" windowHeight="15720" xr2:uid="{9C9A1E89-5FF4-422D-A4F0-75E93BA25FE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9C9A1E89-5FF4-422D-A4F0-75E93BA25FE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Inclusion" sheetId="1" r:id="rId1"/>
-    <sheet name="Dropdown Options" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Dropdown Options" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="98">
   <si>
     <t>Include (Y/N)</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Reason for not including</t>
   </si>
   <si>
-    <t>nIndividualObs</t>
-  </si>
-  <si>
     <t>hasCoordinates</t>
   </si>
   <si>
@@ -57,9 +55,6 @@
     <t>species</t>
   </si>
   <si>
-    <t>ref</t>
-  </si>
-  <si>
     <t>doi</t>
   </si>
   <si>
@@ -229,13 +224,209 @@
   </si>
   <si>
     <t>boscai</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>Baláž, V., M. Solský, D. Lastra González, B. Havlíková, J. Gallego Zamorano, C. González Sevilleja, L. Torrent, and J. Vojar. 2018. First survey of the pathogenic fungus Batrachochytrium salamandrivorans in wild and captive amphibians in the Czech Republic. Salamandra 54:87-91.</t>
+  </si>
+  <si>
+    <t>https://www.salamandra-journal.com/index.php/home/contents/2018-vol-54/1896-balaz-v-m-solsky-d-lastra-gonzalez-b-havlikova-j-gallego-zamorano-c-gonzalez-sevilleja-l-torrent-j-vojar/file</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>CZE</t>
+  </si>
+  <si>
+    <t>include (Y/N)</t>
+  </si>
+  <si>
+    <t>hasCoordinates (Y/N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant table/figure/SI </t>
+  </si>
+  <si>
+    <t>additional comments</t>
+  </si>
+  <si>
+    <t>reason for not including</t>
+  </si>
+  <si>
+    <t>hasDates (Y/N)</t>
+  </si>
+  <si>
+    <t>relevant table/figure/supplement</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Not within confirmed Bsal range; no Bsal+ cases or Bsal related deaths</t>
+  </si>
+  <si>
+    <r>
+      <t>Beukema, W., A. Martel, T. T. Nguyen, K. Goka, D. S. Schmeller, Z. Yuan, A. E. Laking, T. Q. Nguyen, C.-F. Lin, J. Shelton, A. Loyau, F. Pasmans, and B. Wintle. 2018. Environmental context and differences between native and invasive observed niches of</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Batrachochytrium salamandrivorans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> affect invasion risk assessments in the Western Palaearctic. Diversity and Distributions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:1788-1801.</t>
+    </r>
+  </si>
+  <si>
+    <t>Paper has useful comments on Bsal qPCR</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/ddi.12795</t>
+  </si>
+  <si>
+    <t>Figure 1a,c; SI Appendix S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location: Palearctic. </t>
+  </si>
+  <si>
+    <t>Mix of real observations and generated observations; unsure of which is which</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bosch, J., A. Martel, J. Sopniewski, B. Thumsová, C. Ayres, B. C. Scheele, G. Velo-Antón, and F. Pasmans. 2021. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Batrachochytrium salamandrivorans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Threat to the Iberian Urodele Hotspot. Journal of Fungi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:644.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/jof7080644</t>
+  </si>
+  <si>
+    <t>Only some observations have dates</t>
+  </si>
+  <si>
+    <t>data sent from author</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10393-016-1188-7</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>CHE</t>
+  </si>
+  <si>
+    <t>Parrott, J. C., A. Shepack, D. Burkart, B. LaBumbard, P. Scime, E. Baruch, and A. Catenazzi. 2017. Survey of Pathogenic Chytrid Fungi (Batrachochytrium dendrobatidis and B. salamandrivorans) in Salamanders from Three Mountain Ranges in Europe and the Americas. Ecohealth 14:296-302.</t>
+  </si>
+  <si>
+    <t>data from project found on AmphibiaWeb</t>
+  </si>
+  <si>
+    <t>Cunningham, A. A., F. Smith, T. J. McKinley, M. W. Perkins, L. D. Fitzpatrick, O. N. Wright, and B. Lawson. 2019. Apparent absence of Batrachochytrium salamandrivorans in wild urodeles in the United Kingdom. Sci Rep 9:2831.</t>
+  </si>
+  <si>
+    <t>Included in final dataset but not in analyses</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41598-019-39338-4</t>
+  </si>
+  <si>
+    <t>https://shop.laurenti.de/media/ZfF%202018-01-01%20-%20Dalbeck%20et%20al.pdf</t>
+  </si>
+  <si>
+    <t>Dalbeck, L., H. Düssel-Siebert, A. Kerres, K. Kirst, A. Koch, S. Lötters, D. Ohlhoff, J. Sabino-Pinto, K. Preißler, U. Schulte, V. Schulz, S. Steinfartz, M. Veith, M. Vences, N. Wagner, and J. Wegge. 2018. Die Salamanderpest und ihr Erreger Batrachochytrium salamandrivorans (Bsal): aktueller Stand in Deutschland. Zeitschrift für Feldherpetologie 25:1-22.</t>
+  </si>
+  <si>
+    <t>paper link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +436,37 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,13 +489,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,17 +828,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19A25EE-699B-4D58-895E-7B67FDEDB0BC}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUM(31,25,12,8,7,1,2,10, 28)</f>
+        <v>124</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1395</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5">
+        <v>2017</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3">
+        <v>265</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N4" r:id="rId1" xr:uid="{86B61EF4-9CCF-4551-BD6B-8E9EB002E131}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{680ED858-433D-4A69-849D-A6C911D8E6E1}"/>
+    <hyperlink ref="N6" r:id="rId3" xr:uid="{3E7487DD-DBE1-476B-BD2D-ED303DACBDE6}"/>
+    <hyperlink ref="N7" r:id="rId4" xr:uid="{9918273C-BEFE-4242-BD14-8D5A2770A4F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0A3795FF-E0B4-4CD1-9A7A-CE57ECDD4843}">
+          <x14:formula1>
+            <xm:f>'Dropdown Options'!$J$2:$J$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB5190E1-4539-40C5-8F23-FCF0A306929E}">
+          <x14:formula1>
+            <xm:f>'Dropdown Options'!$D$2:$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F5AC4EF-8765-4902-B4D8-CC6779B073BD}">
+          <x14:formula1>
+            <xm:f>'Dropdown Options'!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71B85663-5622-41E9-A5CB-71027F1A6178}">
+          <x14:formula1>
+            <xm:f>'Dropdown Options'!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{142A81EE-3E50-4C54-A566-54B7A9408658}">
+          <x14:formula1>
+            <xm:f>'Dropdown Options'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF984451-B5D0-44C0-8853-0F25F1B94DDE}">
+  <dimension ref="A1:O37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -609,40 +1185,40 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -651,39 +1227,39 @@
         <v>1</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2">
         <v>2015</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K2">
         <v>58</v>
@@ -692,42 +1268,42 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>2014</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K3">
         <v>122</v>
@@ -736,42 +1312,42 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
       </c>
       <c r="E4">
         <v>2016</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K4">
         <v>37</v>
@@ -780,42 +1356,42 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
       </c>
       <c r="E5">
         <v>2016</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K5">
         <v>30</v>
@@ -824,42 +1400,42 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
       </c>
       <c r="E6">
         <v>2016</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K6">
         <v>16</v>
@@ -868,42 +1444,42 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>2016</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K7">
         <v>25</v>
@@ -912,42 +1488,42 @@
         <v>7</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>2016</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K8">
         <v>150</v>
@@ -956,42 +1532,42 @@
         <v>16</v>
       </c>
       <c r="M8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>2016</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K9">
         <v>88</v>
@@ -1000,42 +1576,42 @@
         <v>5</v>
       </c>
       <c r="M9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>2016</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K10">
         <v>10</v>
@@ -1044,42 +1620,42 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>2016</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K11">
         <v>86</v>
@@ -1088,42 +1664,42 @@
         <v>26</v>
       </c>
       <c r="M11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>2016</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K12">
         <v>5</v>
@@ -1132,42 +1708,42 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13">
         <v>2016</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13">
         <v>19</v>
@@ -1176,42 +1752,42 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>2014</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K14">
         <v>233</v>
@@ -1220,42 +1796,42 @@
         <v>25</v>
       </c>
       <c r="M14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>2014</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K15">
         <v>100</v>
@@ -1264,42 +1840,42 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>2014</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K16">
         <v>100</v>
@@ -1308,42 +1884,42 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>2014</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K17">
         <v>7</v>
@@ -1352,42 +1928,42 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <v>2014</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K18">
         <v>35</v>
@@ -1396,42 +1972,42 @@
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>2014</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K19">
         <v>33</v>
@@ -1440,42 +2016,42 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20">
         <v>2014</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K20">
         <v>6</v>
@@ -1484,42 +2060,42 @@
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E21">
         <v>2014</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -1528,42 +2104,42 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22">
         <v>2014</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K22">
         <v>15</v>
@@ -1572,42 +2148,42 @@
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23">
         <v>2014</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K23">
         <v>8</v>
@@ -1616,42 +2192,42 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <v>2014</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K24">
         <v>24</v>
@@ -1660,42 +2236,42 @@
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E25">
         <v>2014</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K25">
         <v>22</v>
@@ -1704,42 +2280,42 @@
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E26">
         <v>2014</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K26">
         <v>73</v>
@@ -1748,42 +2324,42 @@
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27">
         <v>2014</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K27">
         <v>44</v>
@@ -1792,42 +2368,42 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E28">
         <v>2014</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K28">
         <v>2</v>
@@ -1836,42 +2412,42 @@
         <v>0</v>
       </c>
       <c r="M28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E29">
         <v>2014</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K29">
         <v>39</v>
@@ -1880,42 +2456,42 @@
         <v>13</v>
       </c>
       <c r="M29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E30">
         <v>2014</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K30">
         <v>5</v>
@@ -1924,42 +2500,42 @@
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E31">
         <v>2014</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K31">
         <v>5</v>
@@ -1970,277 +2546,259 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E32">
         <v>2014</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E33">
         <v>2014</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E34">
         <v>2014</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E35">
         <v>2014</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E36">
         <v>2014</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E37">
         <v>2014</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{723C89C3-8A7F-4F65-BE56-B9FD8C986590}"/>
+    <hyperlink ref="D30" r:id="rId2" xr:uid="{29D052D0-112C-4287-A0FB-91BE34E98A54}"/>
+    <hyperlink ref="D36" r:id="rId3" xr:uid="{33DED5A9-7D11-4198-A10E-3306D06AC4B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71B85663-5622-41E9-A5CB-71027F1A6178}">
-          <x14:formula1>
-            <xm:f>'Dropdown Options'!$H$2:$H$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB5190E1-4539-40C5-8F23-FCF0A306929E}">
-          <x14:formula1>
-            <xm:f>'Dropdown Options'!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F5AC4EF-8765-4902-B4D8-CC6779B073BD}">
-          <x14:formula1>
-            <xm:f>'Dropdown Options'!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0A3795FF-E0B4-4CD1-9A7A-CE57ECDD4843}">
-          <x14:formula1>
-            <xm:f>'Dropdown Options'!$M$2:$M$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40542C-4F19-4474-8963-22868DD31DBA}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
including iucn richness estimates
</commit_message>
<xml_diff>
--- a/csvFiles/metadata.xlsx
+++ b/csvFiles/metadata.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Chapter-2-Analyses\csvFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FF67A3-BF96-44A0-A7AB-A2D7DBEED01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F440D4D2-779A-4609-A72B-F012D0ABCDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="555" windowWidth="29040" windowHeight="15720" xr2:uid="{9C9A1E89-5FF4-422D-A4F0-75E93BA25FE6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data_Sources" sheetId="3" r:id="rId1"/>
-    <sheet name="Bsal_Occurrence_Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Bsal_Occurrence_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Other_Data_Sources" sheetId="3" r:id="rId2"/>
     <sheet name="Dropdown_Options" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="201">
   <si>
     <t>pubYear</t>
   </si>
@@ -318,9 +318,6 @@
     <t>https://conbio.onlinelibrary.wiley.com/doi/full/10.1111/conl.12436</t>
   </si>
   <si>
-    <t>Contact author for data</t>
-  </si>
-  <si>
     <t>No coordinate data</t>
   </si>
   <si>
@@ -836,12 +833,27 @@
   <si>
     <t>GPM_3IMERGDL</t>
   </si>
+  <si>
+    <t>Contact author(s) for data?</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Other_Data_Sources</t>
+  </si>
+  <si>
+    <t>***PLEASE DO NOT ALTER ANYTHING ON THIS SHEET***</t>
+  </si>
+  <si>
+    <t>dataset_var_name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +927,14 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1034,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1069,14 +1089,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1086,7 +1102,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1094,8 +1109,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1121,13 +1146,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1181,13 +1206,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1536,261 +1561,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40845F99-BD87-4686-8C31-E70A21EEA598}">
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="30">
-        <v>45203</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="O2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>174</v>
-      </c>
-      <c r="K3" s="30">
-        <v>45203</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="O3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G4" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" t="s">
-        <v>179</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>174</v>
-      </c>
-      <c r="K4" s="30">
-        <v>45204</v>
-      </c>
-      <c r="L4" t="s">
-        <v>194</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N4" s="29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{C0BB896B-EADE-4A4B-85C6-794FB9315CB3}"/>
-    <hyperlink ref="M3" r:id="rId2" xr:uid="{44A967CD-C865-4B7B-A59C-F17F73B8D1AC}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{04A6F5EF-C9F8-4E08-88BA-C7C4257ACA2D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1E04F19-736C-4E89-9F74-41BE674085D8}">
-          <x14:formula1>
-            <xm:f>Dropdown_Options!$D$7:$D$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B56B37C-050F-4B38-A768-6EE58101C50A}">
-          <x14:formula1>
-            <xm:f>Dropdown_Options!$E$7:$E$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9771DD4E-223A-4F9F-AD5D-5B9DCE1D9200}">
-          <x14:formula1>
-            <xm:f>Dropdown_Options!$G$7:$G$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4F1ECE3-1E5D-46EA-8A37-37B3674BA6B8}">
-          <x14:formula1>
-            <xm:f>Dropdown_Options!$I$7:$I$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19A25EE-699B-4D58-895E-7B67FDEDB0BC}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,7 +1589,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1822,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>9</v>
@@ -1831,28 +1607,28 @@
         <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1887,16 +1663,16 @@
         <v>36</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
         <v>63</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1928,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>16</v>
@@ -1940,7 +1716,7 @@
         <v>43</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2029,7 +1805,7 @@
         <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2070,7 +1846,7 @@
         <v>24</v>
       </c>
       <c r="N6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2164,10 +1940,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
       </c>
       <c r="C9">
         <v>2016</v>
@@ -2191,27 +1967,27 @@
         <v>3</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" t="s">
         <v>48</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="N9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
       </c>
       <c r="C10">
         <v>2016</v>
@@ -2233,19 +2009,19 @@
         <v>3</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="L10" t="s">
         <v>55</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2276,10 +2052,10 @@
         <v>3</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
         <v>35</v>
@@ -2288,7 +2064,7 @@
         <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2320,24 +2096,24 @@
         <v>2</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="N12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" t="s">
-        <v>66</v>
       </c>
       <c r="C13">
         <v>2022</v>
@@ -2364,21 +2140,21 @@
         <v>36</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" t="s">
         <v>68</v>
-      </c>
-      <c r="N13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>22</v>
@@ -2405,19 +2181,19 @@
         <v>3</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="L14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2449,16 +2225,16 @@
         <v>2</v>
       </c>
       <c r="K15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" t="s">
+        <v>77</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" t="s">
         <v>81</v>
-      </c>
-      <c r="L15" t="s">
-        <v>78</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N15" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2490,16 +2266,16 @@
         <v>2</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="N16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2531,16 +2307,16 @@
         <v>2</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2568,16 +2344,16 @@
         <v>2</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" t="s">
         <v>92</v>
-      </c>
-      <c r="N18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -2609,16 +2385,16 @@
         <v>3</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="L19" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2650,13 +2426,13 @@
         <v>2</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2691,21 +2467,21 @@
         <v>16</v>
       </c>
       <c r="L21" t="s">
+        <v>101</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" t="s">
         <v>102</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
         <v>104</v>
-      </c>
-      <c r="B22" t="s">
-        <v>105</v>
       </c>
       <c r="C22">
         <v>2019</v>
@@ -2735,18 +2511,18 @@
         <v>16</v>
       </c>
       <c r="L22" t="s">
+        <v>105</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23">
         <v>2022</v>
@@ -2773,21 +2549,21 @@
         <v>36</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L23" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
         <v>114</v>
-      </c>
-      <c r="B24" t="s">
-        <v>115</v>
       </c>
       <c r="C24">
         <v>2022</v>
@@ -2817,21 +2593,21 @@
         <v>16</v>
       </c>
       <c r="L24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N24" t="s">
         <v>116</v>
-      </c>
-      <c r="N24" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" t="s">
         <v>120</v>
-      </c>
-      <c r="B25" t="s">
-        <v>121</v>
       </c>
       <c r="C25">
         <v>2020</v>
@@ -2855,24 +2631,24 @@
         <v>3</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L25" t="s">
+        <v>117</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="N25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
         <v>125</v>
-      </c>
-      <c r="B26" t="s">
-        <v>126</v>
       </c>
       <c r="C26">
         <v>2021</v>
@@ -2899,13 +2675,13 @@
         <v>36</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2938,24 +2714,24 @@
         <v>2</v>
       </c>
       <c r="K27" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="L27" t="s">
+        <v>129</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N27" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="L27" t="s">
-        <v>130</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28">
         <v>2017</v>
@@ -2979,19 +2755,19 @@
         <v>3</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="L28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="N28" s="14" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3037,25 +2813,25 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{142A81EE-3E50-4C54-A566-54B7A9408658}">
           <x14:formula1>
-            <xm:f>Dropdown_Options!$E$2:$E$3</xm:f>
+            <xm:f>Dropdown_Options!$E$3:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F5AC4EF-8765-4902-B4D8-CC6779B073BD}">
           <x14:formula1>
-            <xm:f>Dropdown_Options!$G$2:$G$3</xm:f>
+            <xm:f>Dropdown_Options!$G$3:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0A3795FF-E0B4-4CD1-9A7A-CE57ECDD4843}">
           <x14:formula1>
-            <xm:f>Dropdown_Options!$I$2:$I$3</xm:f>
+            <xm:f>Dropdown_Options!$I$3:$I$4</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71B85663-5622-41E9-A5CB-71027F1A6178}">
           <x14:formula1>
-            <xm:f>Dropdown_Options!$H$2:$H$3</xm:f>
+            <xm:f>Dropdown_Options!$H$3:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
@@ -3065,224 +2841,557 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40845F99-BD87-4686-8C31-E70A21EEA598}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="27">
+        <v>45203</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="27">
+        <v>45203</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N3" t="s">
+        <v>176</v>
+      </c>
+      <c r="O3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" s="27">
+        <v>45204</v>
+      </c>
+      <c r="L4" t="s">
+        <v>193</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{C0BB896B-EADE-4A4B-85C6-794FB9315CB3}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{44A967CD-C865-4B7B-A59C-F17F73B8D1AC}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{04A6F5EF-C9F8-4E08-88BA-C7C4257ACA2D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1E04F19-736C-4E89-9F74-41BE674085D8}">
+          <x14:formula1>
+            <xm:f>Dropdown_Options!$D$8:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B56B37C-050F-4B38-A768-6EE58101C50A}">
+          <x14:formula1>
+            <xm:f>Dropdown_Options!$E$8:$E$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9771DD4E-223A-4F9F-AD5D-5B9DCE1D9200}">
+          <x14:formula1>
+            <xm:f>Dropdown_Options!$G$8:$G$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4F1ECE3-1E5D-46EA-8A37-37B3674BA6B8}">
+          <x14:formula1>
+            <xm:f>Dropdown_Options!$I$8:$I$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40542C-4F19-4474-8963-22868DD31DBA}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="25" t="s">
+      <c r="M2" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+      <c r="R2" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="18"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="6" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="E7" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="G7" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="K7" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="O7" s="32"/>
+      <c r="P7" s="33"/>
+      <c r="R7" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N6" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="F10" s="30"/>
+      <c r="G10" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" s="18" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G10" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="18" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G11" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="21"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:S1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>